<commit_message>
agregar subida de información acerca de descarga y retiro de puerto
</commit_message>
<xml_diff>
--- a/secuencias/sti/A.P. MOLLER.xlsx
+++ b/secuencias/sti/A.P. MOLLER.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Sigla</t>
   </si>
@@ -52,12 +52,6 @@
     <t>ETA</t>
   </si>
   <si>
-    <t>TCKU</t>
-  </si>
-  <si>
-    <t>MRSU</t>
-  </si>
-  <si>
     <t>MRKU</t>
   </si>
   <si>
@@ -71,18 +65,6 @@
   </si>
   <si>
     <t>NO</t>
-  </si>
-  <si>
-    <t>10/11/2023  17:30</t>
-  </si>
-  <si>
-    <t>10/11/2023  18:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02/11/2023 01:29 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">02/11/2023 01:45 </t>
   </si>
   <si>
     <t xml:space="preserve">02/11/2023 17:06 </t>
@@ -449,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -498,101 +480,31 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>653150</v>
+        <v>701925</v>
       </c>
       <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
-        <v>467359</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <v>701925</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>